<commit_message>
modified:   IBAv2.py 	modified:   system/iba_google_credential 	new file:   system/private.ppk 	new file:   system/public 	new file:   system/sql_abfrage_installationsdaten.sql 	new file:   system/sql_abfrage_installationsdatenv2.sql 	new file:   system/sql_abfrage_installationsdatenv3.sql 	new file:   system/sql_abfrage_installationsdatenv4.sql 	modified:   system/was_liegt_wo.xlsx Safety First
</commit_message>
<xml_diff>
--- a/system/was_liegt_wo.xlsx
+++ b/system/was_liegt_wo.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="112">
   <si>
     <t>Bezeichner</t>
   </si>
@@ -269,9 +269,6 @@
     <t>C:\Users\RobertM\Desktop\db_exceldateien\EVA.xlsx</t>
   </si>
   <si>
-    <t>unklar</t>
-  </si>
-  <si>
     <t>MST.xls</t>
   </si>
   <si>
@@ -279,13 +276,97 @@
   </si>
   <si>
     <t>Komplex.xls</t>
+  </si>
+  <si>
+    <t>Planungsdaten</t>
+  </si>
+  <si>
+    <t>dbfrontend_messstelle.hinweise_zugang</t>
+  </si>
+  <si>
+    <t>dbfrontend_person.nachname</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>dbfrontend_messstelle.zaehler_vorher</t>
+  </si>
+  <si>
+    <t>dbfrontend_messstelle.msb_vorher</t>
+  </si>
+  <si>
+    <t>dbfrontend_messstelle.spannung_ungewandelt</t>
+  </si>
+  <si>
+    <t>dbfrontend_messstelle.spannung_gewandelt</t>
+  </si>
+  <si>
+    <t>dbfrontend_messstelle.strom_ungewandelt</t>
+  </si>
+  <si>
+    <t>dbfrontend_messstelle.strom_gewandelt</t>
+  </si>
+  <si>
+    <t>Steuerstelle Excel</t>
+  </si>
+  <si>
+    <t>Nummer MST/STST</t>
+  </si>
+  <si>
+    <t>Datum Installation</t>
+  </si>
+  <si>
+    <t>Auftrag Messstelle</t>
+  </si>
+  <si>
+    <t>Auftrag Steuerstelle</t>
+  </si>
+  <si>
+    <t>Termin angefragt bei</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nachname / Vorname </t>
+  </si>
+  <si>
+    <t>Telefon</t>
+  </si>
+  <si>
+    <t>evtl. eindeutige Spaltenbezeichnung</t>
+  </si>
+  <si>
+    <t>Mobil</t>
+  </si>
+  <si>
+    <t>Ausbau Altzähler durch</t>
+  </si>
+  <si>
+    <t>Typenschlüssen (Anfang)</t>
+  </si>
+  <si>
+    <t>Spannung</t>
+  </si>
+  <si>
+    <t>Stromtyp</t>
+  </si>
+  <si>
+    <t>Genauigkeitsklasse</t>
+  </si>
+  <si>
+    <t>Bezeichnung</t>
+  </si>
+  <si>
+    <t>technische Hinweise Messstelle</t>
+  </si>
+  <si>
+    <t>technische Hinweise Steuerstelle</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -321,8 +402,23 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -359,8 +455,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -383,13 +489,30 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -410,11 +533,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="2" xfId="4"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="3" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="1" xfId="4" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="5">
+    <cellStyle name="Berechnung" xfId="4" builtinId="22"/>
+    <cellStyle name="Schlecht" xfId="3" builtinId="27"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
     <cellStyle name="Standard 2" xfId="1"/>
     <cellStyle name="Standard 3" xfId="2"/>
@@ -732,42 +862,42 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:J60"/>
+  <dimension ref="A1:J1048576"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B19" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="G11" sqref="G11"/>
+      <selection pane="bottomRight" activeCell="O30" sqref="O30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="25.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="13.7109375" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="14" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="18" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="23.5703125" hidden="1" customWidth="1"/>
     <col min="9" max="9" width="43.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="18" t="s">
         <v>58</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14" t="s">
+      <c r="B1" s="18"/>
+      <c r="C1" s="18" t="s">
         <v>59</v>
       </c>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
-      <c r="H1" s="14" t="s">
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18" t="s">
         <v>61</v>
       </c>
-      <c r="I1" s="14"/>
+      <c r="I1" s="18"/>
       <c r="J1" s="2"/>
     </row>
     <row r="2" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -777,13 +907,13 @@
         <v>60</v>
       </c>
       <c r="D2" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="E2" s="11" t="s">
         <v>82</v>
       </c>
-      <c r="E2" s="11" t="s">
+      <c r="F2" s="11" t="s">
         <v>83</v>
-      </c>
-      <c r="F2" s="11" t="s">
-        <v>84</v>
       </c>
       <c r="G2" s="11" t="s">
         <v>74</v>
@@ -825,7 +955,9 @@
       <c r="F4" s="11"/>
       <c r="G4" s="11"/>
       <c r="H4" s="11"/>
-      <c r="I4" s="10"/>
+      <c r="I4" s="10" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
@@ -842,7 +974,7 @@
       <c r="H5" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="I5" s="10" t="s">
+      <c r="I5" s="14" t="s">
         <v>62</v>
       </c>
     </row>
@@ -863,7 +995,7 @@
       <c r="H6" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="I6" s="10" t="s">
+      <c r="I6" s="14" t="s">
         <v>63</v>
       </c>
     </row>
@@ -884,7 +1016,7 @@
       <c r="H7" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="I7" s="10" t="s">
+      <c r="I7" s="14" t="s">
         <v>64</v>
       </c>
     </row>
@@ -905,7 +1037,7 @@
       <c r="H8" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="I8" s="10" t="s">
+      <c r="I8" s="14" t="s">
         <v>65</v>
       </c>
     </row>
@@ -924,7 +1056,7 @@
       <c r="H9" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="I9" s="10" t="s">
+      <c r="I9" s="14" t="s">
         <v>66</v>
       </c>
     </row>
@@ -941,7 +1073,9 @@
       <c r="F10" s="11"/>
       <c r="G10" s="11"/>
       <c r="H10" s="11"/>
-      <c r="I10" s="10"/>
+      <c r="I10" s="10" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
@@ -956,7 +1090,9 @@
       <c r="F11" s="10"/>
       <c r="G11" s="10"/>
       <c r="H11" s="10"/>
-      <c r="I11" s="10"/>
+      <c r="I11" s="10" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
@@ -971,7 +1107,9 @@
       <c r="F12" s="10"/>
       <c r="G12" s="10"/>
       <c r="H12" s="10"/>
-      <c r="I12" s="10"/>
+      <c r="I12" s="10" t="s">
+        <v>97</v>
+      </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
@@ -986,7 +1124,9 @@
       <c r="F13" s="10"/>
       <c r="G13" s="10"/>
       <c r="H13" s="10"/>
-      <c r="I13" s="10"/>
+      <c r="I13" s="10" t="s">
+        <v>98</v>
+      </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
@@ -1001,7 +1141,9 @@
       <c r="F14" s="10"/>
       <c r="G14" s="10"/>
       <c r="H14" s="10"/>
-      <c r="I14" s="10"/>
+      <c r="I14" s="10" t="s">
+        <v>99</v>
+      </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
@@ -1020,7 +1162,7 @@
       <c r="H15" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="I15" s="10" t="s">
+      <c r="I15" s="14" t="s">
         <v>67</v>
       </c>
     </row>
@@ -1041,11 +1183,11 @@
       <c r="H16" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="I16" s="10" t="s">
+      <c r="I16" s="14" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
         <v>14</v>
       </c>
@@ -1062,11 +1204,11 @@
       <c r="H17" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="I17" s="10" t="s">
+      <c r="I17" s="14" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
         <v>15</v>
       </c>
@@ -1083,11 +1225,11 @@
       <c r="H18" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="I18" s="10" t="s">
+      <c r="I18" s="14" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
         <v>16</v>
       </c>
@@ -1104,9 +1246,14 @@
       <c r="F19" s="10"/>
       <c r="G19" s="10"/>
       <c r="H19" s="10"/>
-      <c r="I19" s="10"/>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I19" s="19" t="s">
+        <v>84</v>
+      </c>
+      <c r="J19" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
         <v>17</v>
       </c>
@@ -1121,11 +1268,11 @@
       <c r="H20" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="I20" s="10" t="s">
+      <c r="I20" s="14" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
         <v>18</v>
       </c>
@@ -1140,9 +1287,14 @@
       </c>
       <c r="G21" s="10"/>
       <c r="H21" s="10"/>
-      <c r="I21" s="10"/>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I21" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="J21" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
         <v>19</v>
       </c>
@@ -1157,9 +1309,14 @@
       </c>
       <c r="G22" s="10"/>
       <c r="H22" s="10"/>
-      <c r="I22" s="10"/>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I22" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="J22" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
         <v>20</v>
       </c>
@@ -1174,9 +1331,14 @@
       </c>
       <c r="G23" s="10"/>
       <c r="H23" s="10"/>
-      <c r="I23" s="10"/>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I23" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="J23" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
         <v>21</v>
       </c>
@@ -1189,9 +1351,11 @@
       <c r="F24" s="12"/>
       <c r="G24" s="12"/>
       <c r="H24" s="10"/>
-      <c r="I24" s="10"/>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I24" s="14" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
         <v>22</v>
       </c>
@@ -1208,11 +1372,11 @@
       <c r="H25" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="I25" s="10" t="s">
+      <c r="I25" s="14" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
         <v>23</v>
       </c>
@@ -1225,9 +1389,14 @@
       <c r="F26" s="10"/>
       <c r="G26" s="10"/>
       <c r="H26" s="10"/>
-      <c r="I26" s="10"/>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I26" s="19" t="s">
+        <v>84</v>
+      </c>
+      <c r="J26" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>24</v>
       </c>
@@ -1242,11 +1411,11 @@
       <c r="H27" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="I27" s="10" t="s">
+      <c r="I27" s="14" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>25</v>
       </c>
@@ -1261,9 +1430,11 @@
       <c r="F28" s="10"/>
       <c r="G28" s="10"/>
       <c r="H28" s="10"/>
-      <c r="I28" s="10"/>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I28" s="14" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>26</v>
       </c>
@@ -1278,9 +1449,11 @@
       <c r="F29" s="10"/>
       <c r="G29" s="10"/>
       <c r="H29" s="10"/>
-      <c r="I29" s="10"/>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I29" s="14" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>27</v>
       </c>
@@ -1295,9 +1468,11 @@
       <c r="F30" s="10"/>
       <c r="G30" s="10"/>
       <c r="H30" s="10"/>
-      <c r="I30" s="10"/>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I30" s="14" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>28</v>
       </c>
@@ -1312,9 +1487,11 @@
       <c r="F31" s="10"/>
       <c r="G31" s="10"/>
       <c r="H31" s="10"/>
-      <c r="I31" s="10"/>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I31" s="14" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
         <v>29</v>
       </c>
@@ -1329,9 +1506,11 @@
       <c r="F32" s="10"/>
       <c r="G32" s="10"/>
       <c r="H32" s="10"/>
-      <c r="I32" s="10"/>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I32" s="14" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
         <v>30</v>
       </c>
@@ -1346,9 +1525,11 @@
       <c r="F33" s="10"/>
       <c r="G33" s="10"/>
       <c r="H33" s="10"/>
-      <c r="I33" s="10"/>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I33" s="14" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
         <v>31</v>
       </c>
@@ -1363,9 +1544,11 @@
       <c r="F34" s="10"/>
       <c r="G34" s="10"/>
       <c r="H34" s="10"/>
-      <c r="I34" s="10"/>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I34" s="14" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="8" t="s">
         <v>32</v>
       </c>
@@ -1381,8 +1564,11 @@
       </c>
       <c r="H35" s="10"/>
       <c r="I35" s="10"/>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J35" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
         <v>33</v>
       </c>
@@ -1395,9 +1581,11 @@
       <c r="F36" s="10"/>
       <c r="G36" s="10"/>
       <c r="H36" s="10"/>
-      <c r="I36" s="10"/>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I36" s="10" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
         <v>34</v>
       </c>
@@ -1412,11 +1600,11 @@
       <c r="H37" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="I37" s="10" t="s">
+      <c r="I37" s="14" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
         <v>35</v>
       </c>
@@ -1431,9 +1619,11 @@
       <c r="F38" s="10"/>
       <c r="G38" s="10"/>
       <c r="H38" s="10"/>
-      <c r="I38" s="10"/>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I38" s="14" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
         <v>36</v>
       </c>
@@ -1448,9 +1638,11 @@
       <c r="F39" s="10"/>
       <c r="G39" s="10"/>
       <c r="H39" s="10"/>
-      <c r="I39" s="10"/>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I39" s="14" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
         <v>37</v>
       </c>
@@ -1465,9 +1657,11 @@
       <c r="F40" s="10"/>
       <c r="G40" s="10"/>
       <c r="H40" s="10"/>
-      <c r="I40" s="10"/>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I40" s="14" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
         <v>38</v>
       </c>
@@ -1482,9 +1676,11 @@
       <c r="F41" s="10"/>
       <c r="G41" s="10"/>
       <c r="H41" s="10"/>
-      <c r="I41" s="10"/>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I41" s="14" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
         <v>39</v>
       </c>
@@ -1497,9 +1693,11 @@
       <c r="F42" s="10"/>
       <c r="G42" s="10"/>
       <c r="H42" s="10"/>
-      <c r="I42" s="10"/>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I42" s="10" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
         <v>40</v>
       </c>
@@ -1514,9 +1712,11 @@
       <c r="F43" s="10"/>
       <c r="G43" s="10"/>
       <c r="H43" s="10"/>
-      <c r="I43" s="10"/>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I43" s="10" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
         <v>41</v>
       </c>
@@ -1529,9 +1729,11 @@
       <c r="F44" s="10"/>
       <c r="G44" s="10"/>
       <c r="H44" s="10"/>
-      <c r="I44" s="10"/>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I44" s="10" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
         <v>42</v>
       </c>
@@ -1544,9 +1746,11 @@
       <c r="F45" s="10"/>
       <c r="G45" s="10"/>
       <c r="H45" s="10"/>
-      <c r="I45" s="10"/>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I45" s="10" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
         <v>43</v>
       </c>
@@ -1561,9 +1765,11 @@
       <c r="F46" s="10"/>
       <c r="G46" s="10"/>
       <c r="H46" s="10"/>
-      <c r="I46" s="10"/>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I46" s="10" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
         <v>44</v>
       </c>
@@ -1578,9 +1784,11 @@
       <c r="F47" s="10"/>
       <c r="G47" s="10"/>
       <c r="H47" s="10"/>
-      <c r="I47" s="10"/>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I47" s="10" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
         <v>45</v>
       </c>
@@ -1595,9 +1803,11 @@
       <c r="F48" s="10"/>
       <c r="G48" s="10"/>
       <c r="H48" s="10"/>
-      <c r="I48" s="10"/>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I48" s="10" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
         <v>46</v>
       </c>
@@ -1610,9 +1820,14 @@
       <c r="F49" s="10"/>
       <c r="G49" s="10"/>
       <c r="H49" s="10"/>
-      <c r="I49" s="10"/>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I49" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="J49" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" s="8" t="s">
         <v>47</v>
       </c>
@@ -1625,9 +1840,14 @@
       <c r="F50" s="12"/>
       <c r="G50" s="12"/>
       <c r="H50" s="10"/>
-      <c r="I50" s="10"/>
-    </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I50" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="J50" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
         <v>48</v>
       </c>
@@ -1642,9 +1862,11 @@
       <c r="F51" s="10"/>
       <c r="G51" s="10"/>
       <c r="H51" s="10"/>
-      <c r="I51" s="10"/>
-    </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I51" s="10" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" s="7" t="s">
         <v>49</v>
       </c>
@@ -1661,11 +1883,14 @@
       <c r="H52" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="I52" s="10" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I52" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="J52" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" s="7" t="s">
         <v>50</v>
       </c>
@@ -1680,11 +1905,14 @@
       <c r="F53" s="10"/>
       <c r="G53" s="10"/>
       <c r="H53" s="10"/>
-      <c r="I53" s="10" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I53" s="17" t="s">
+        <v>68</v>
+      </c>
+      <c r="J53" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" s="7" t="s">
         <v>51</v>
       </c>
@@ -1699,11 +1927,14 @@
       <c r="F54" s="10"/>
       <c r="G54" s="10"/>
       <c r="H54" s="10"/>
-      <c r="I54" s="10" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I54" s="17" t="s">
+        <v>69</v>
+      </c>
+      <c r="J54" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" s="7" t="s">
         <v>52</v>
       </c>
@@ -1718,11 +1949,14 @@
       <c r="F55" s="10"/>
       <c r="G55" s="10"/>
       <c r="H55" s="10"/>
-      <c r="I55" s="10" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I55" s="17" t="s">
+        <v>70</v>
+      </c>
+      <c r="J55" s="15" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" s="7" t="s">
         <v>53</v>
       </c>
@@ -1737,9 +1971,11 @@
       <c r="F56" s="10"/>
       <c r="G56" s="10"/>
       <c r="H56" s="10"/>
-      <c r="I56" s="10"/>
-    </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I56" s="16" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" s="7" t="s">
         <v>54</v>
       </c>
@@ -1754,9 +1990,11 @@
       <c r="F57" s="10"/>
       <c r="G57" s="10"/>
       <c r="H57" s="10"/>
-      <c r="I57" s="10"/>
-    </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I57" s="16" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" s="7" t="s">
         <v>55</v>
       </c>
@@ -1769,9 +2007,11 @@
       <c r="F58" s="10"/>
       <c r="G58" s="10"/>
       <c r="H58" s="10"/>
-      <c r="I58" s="10"/>
-    </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I58" s="10" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" s="7" t="s">
         <v>56</v>
       </c>
@@ -1784,9 +2024,11 @@
       <c r="F59" s="10"/>
       <c r="G59" s="10"/>
       <c r="H59" s="10"/>
-      <c r="I59" s="10"/>
-    </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I59" s="10" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" s="7" t="s">
         <v>57</v>
       </c>
@@ -1801,7 +2043,14 @@
       <c r="F60" s="10"/>
       <c r="G60" s="10"/>
       <c r="H60" s="10"/>
-      <c r="I60" s="10"/>
+      <c r="I60" s="10" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="1048576" spans="10:10" x14ac:dyDescent="0.25">
+      <c r="J1048576" s="1" t="s">
+        <v>87</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -1810,6 +2059,6 @@
     <mergeCell ref="H1:I1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="54" orientation="landscape" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="10" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>